<commit_message>
Added 2021 styles Fixed error handling for 550 error when existing file found Updated alert to direct viewers to the styles of the month.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2b05\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:40009_{60F62788-76A3-4AF9-B9B3-0AD1796CD7C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{221F3A70-E47C-4BF1-8CB6-3A879D6AE9C2}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:40009_{60F62788-76A3-4AF9-B9B3-0AD1796CD7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C7AE402-CDB8-4315-A5F7-F5A321090909}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Competitions" sheetId="2" r:id="rId1"/>
@@ -25,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="142">
   <si>
     <t>Date</t>
   </si>
@@ -139,6 +140,9 @@
     <t>Mead and Cider</t>
   </si>
   <si>
+    <t>Mead and Fruit Beers</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -452,6 +456,9 @@
   </si>
   <si>
     <t>Belgian Quad</t>
+  </si>
+  <si>
+    <t>John</t>
   </si>
 </sst>
 </file>
@@ -1008,8 +1015,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:D37" totalsRowShown="0">
-  <autoFilter ref="A1:D37" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:D43" totalsRowShown="0">
+  <autoFilter ref="A1:D43" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Style"/>
@@ -1021,8 +1028,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A1:D119" totalsRowShown="0">
-  <autoFilter ref="A1:D119" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A1:D123" totalsRowShown="0">
+  <autoFilter ref="A1:D123" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name"/>
@@ -1034,8 +1041,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1" displayName="Table1" ref="A1:A22" totalsRowShown="0">
-  <autoFilter ref="A1:A22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1" displayName="Table1" ref="A1:A23" totalsRowShown="0">
+  <autoFilter ref="A1:A23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Name"/>
   </tableColumns>
@@ -1340,15 +1347,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
@@ -1869,6 +1876,90 @@
         <v>24</v>
       </c>
       <c r="D37">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>44392</v>
+      </c>
+      <c r="B38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>44418</v>
+      </c>
+      <c r="B39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>44453</v>
+      </c>
+      <c r="B40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>44481</v>
+      </c>
+      <c r="B41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>44509</v>
+      </c>
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>44544</v>
+      </c>
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43">
         <v>2015</v>
       </c>
     </row>
@@ -1882,10 +1973,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1901,13 +1992,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1915,10 +2006,10 @@
         <v>43109</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -1929,10 +2020,10 @@
         <v>43109</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1943,10 +2034,10 @@
         <v>43109</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1957,7 +2048,7 @@
         <v>43109</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>0.5</v>
@@ -1968,7 +2059,7 @@
         <v>43109</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D6">
         <v>0.5</v>
@@ -1979,10 +2070,10 @@
         <v>43137</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -1993,10 +2084,10 @@
         <v>43137</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -2007,10 +2098,10 @@
         <v>43137</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2021,10 +2112,10 @@
         <v>43172</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -2035,10 +2126,10 @@
         <v>43172</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -2049,10 +2140,10 @@
         <v>43172</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2063,7 +2154,7 @@
         <v>43172</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13">
         <v>0.5</v>
@@ -2074,10 +2165,10 @@
         <v>43200</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -2088,10 +2179,10 @@
         <v>43200</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -2102,10 +2193,10 @@
         <v>43235</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -2116,10 +2207,10 @@
         <v>43235</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -2130,10 +2221,10 @@
         <v>43235</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -2144,7 +2235,7 @@
         <v>43235</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D19">
         <v>0.5</v>
@@ -2155,7 +2246,7 @@
         <v>43235</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D20">
         <v>0.5</v>
@@ -2166,7 +2257,7 @@
         <v>43235</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D21">
         <v>0.5</v>
@@ -2177,7 +2268,7 @@
         <v>43235</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D22">
         <v>0.5</v>
@@ -2188,7 +2279,7 @@
         <v>43235</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D23">
         <v>0.5</v>
@@ -2199,7 +2290,7 @@
         <v>43235</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D24">
         <v>0.5</v>
@@ -2210,10 +2301,10 @@
         <v>43263</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -2224,10 +2315,10 @@
         <v>43263</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -2238,10 +2329,10 @@
         <v>43263</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -2252,7 +2343,7 @@
         <v>43263</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D28">
         <v>0.5</v>
@@ -2263,7 +2354,7 @@
         <v>43263</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D29">
         <v>0.5</v>
@@ -2274,10 +2365,10 @@
         <v>43291</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -2288,10 +2379,10 @@
         <v>43291</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -2302,10 +2393,10 @@
         <v>43291</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -2316,10 +2407,10 @@
         <v>43326</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -2330,10 +2421,10 @@
         <v>43326</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -2344,10 +2435,10 @@
         <v>43326</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -2358,10 +2449,10 @@
         <v>43382</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -2372,7 +2463,7 @@
         <v>43326</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D37">
         <v>0.5</v>
@@ -2383,7 +2474,7 @@
         <v>43326</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D38">
         <v>0.5</v>
@@ -2394,7 +2485,7 @@
         <v>43326</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D39">
         <v>0.5</v>
@@ -2405,7 +2496,7 @@
         <v>43326</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D40">
         <v>0.5</v>
@@ -2416,7 +2507,7 @@
         <v>43326</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D41">
         <v>0.5</v>
@@ -2427,7 +2518,7 @@
         <v>43326</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D42">
         <v>0.5</v>
@@ -2438,10 +2529,10 @@
         <v>43382</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D43">
         <v>2</v>
@@ -2452,10 +2543,10 @@
         <v>43382</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -2466,10 +2557,10 @@
         <v>43382</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D45">
         <v>0.5</v>
@@ -2480,10 +2571,10 @@
         <v>43354</v>
       </c>
       <c r="B46" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D46">
         <v>3</v>
@@ -2494,10 +2585,10 @@
         <v>43473</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D47">
         <v>3</v>
@@ -2508,10 +2599,10 @@
         <v>43473</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D48">
         <v>2</v>
@@ -2522,10 +2613,10 @@
         <v>43473</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -2536,10 +2627,10 @@
         <v>43473</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D50">
         <v>0.5</v>
@@ -2550,10 +2641,10 @@
         <v>43473</v>
       </c>
       <c r="B51" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C51" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D51">
         <v>0.5</v>
@@ -2564,10 +2655,10 @@
         <v>43473</v>
       </c>
       <c r="B52" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C52" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D52">
         <v>0.5</v>
@@ -2578,10 +2669,10 @@
         <v>43508</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D53">
         <v>3</v>
@@ -2592,10 +2683,10 @@
         <v>43508</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C54" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -2606,10 +2697,10 @@
         <v>43536</v>
       </c>
       <c r="B55" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C55" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D55">
         <v>3</v>
@@ -2620,10 +2711,10 @@
         <v>43536</v>
       </c>
       <c r="B56" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C56" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D56">
         <v>2</v>
@@ -2634,10 +2725,10 @@
         <v>43536</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C57" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -2648,10 +2739,10 @@
         <v>43536</v>
       </c>
       <c r="B58" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C58" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D58">
         <v>0.5</v>
@@ -2662,10 +2753,10 @@
         <v>43536</v>
       </c>
       <c r="B59" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C59" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D59">
         <v>0.5</v>
@@ -2676,10 +2767,10 @@
         <v>43627</v>
       </c>
       <c r="B60" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D60">
         <v>3</v>
@@ -2690,10 +2781,10 @@
         <v>43627</v>
       </c>
       <c r="B61" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C61" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -2704,10 +2795,10 @@
         <v>43627</v>
       </c>
       <c r="B62" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C62" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -2718,10 +2809,10 @@
         <v>43627</v>
       </c>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C63" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D63">
         <v>0.5</v>
@@ -2732,10 +2823,10 @@
         <v>43627</v>
       </c>
       <c r="B64" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C64" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D64">
         <v>0.5</v>
@@ -2746,10 +2837,10 @@
         <v>43627</v>
       </c>
       <c r="B65" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C65" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D65">
         <v>0.5</v>
@@ -2760,10 +2851,10 @@
         <v>43627</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C66" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D66">
         <v>0.5</v>
@@ -2774,10 +2865,10 @@
         <v>43627</v>
       </c>
       <c r="B67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C67" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D67">
         <v>0.5</v>
@@ -2788,10 +2879,10 @@
         <v>43627</v>
       </c>
       <c r="B68" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C68" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D68">
         <v>0.5</v>
@@ -2802,10 +2893,10 @@
         <v>43627</v>
       </c>
       <c r="B69" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C69" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D69">
         <v>0.5</v>
@@ -2816,10 +2907,10 @@
         <v>43655</v>
       </c>
       <c r="B70" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C70" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D70">
         <v>3</v>
@@ -2830,10 +2921,10 @@
         <v>43655</v>
       </c>
       <c r="B71" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C71" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D71">
         <v>2</v>
@@ -2844,10 +2935,10 @@
         <v>43655</v>
       </c>
       <c r="B72" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C72" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -2858,10 +2949,10 @@
         <v>43655</v>
       </c>
       <c r="B73" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C73" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D73">
         <v>0.5</v>
@@ -2872,10 +2963,10 @@
         <v>43690</v>
       </c>
       <c r="B74" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C74" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D74">
         <v>3</v>
@@ -2886,10 +2977,10 @@
         <v>43690</v>
       </c>
       <c r="B75" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C75" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D75">
         <v>2</v>
@@ -2900,10 +2991,10 @@
         <v>43690</v>
       </c>
       <c r="B76" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C76" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -2914,10 +3005,10 @@
         <v>43690</v>
       </c>
       <c r="B77" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C77" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D77">
         <v>0.5</v>
@@ -2928,10 +3019,10 @@
         <v>43690</v>
       </c>
       <c r="B78" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C78" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D78">
         <v>0.5</v>
@@ -2942,10 +3033,10 @@
         <v>43690</v>
       </c>
       <c r="B79" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C79" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D79">
         <v>0.5</v>
@@ -2956,10 +3047,10 @@
         <v>43690</v>
       </c>
       <c r="B80" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C80" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D80">
         <v>0.5</v>
@@ -2970,10 +3061,10 @@
         <v>43718</v>
       </c>
       <c r="B81" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C81" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D81">
         <v>3</v>
@@ -2984,10 +3075,10 @@
         <v>43718</v>
       </c>
       <c r="B82" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C82" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D82">
         <v>2</v>
@@ -2998,10 +3089,10 @@
         <v>43718</v>
       </c>
       <c r="B83" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C83" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -3012,10 +3103,10 @@
         <v>43718</v>
       </c>
       <c r="B84" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C84" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D84">
         <v>0.5</v>
@@ -3026,10 +3117,10 @@
         <v>43718</v>
       </c>
       <c r="B85" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C85" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D85">
         <v>0.5</v>
@@ -3040,10 +3131,10 @@
         <v>43718</v>
       </c>
       <c r="B86" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C86" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D86">
         <v>0.5</v>
@@ -3054,10 +3145,10 @@
         <v>43746</v>
       </c>
       <c r="B87" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C87" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D87">
         <v>3</v>
@@ -3068,10 +3159,10 @@
         <v>43746</v>
       </c>
       <c r="B88" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C88" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D88">
         <v>2</v>
@@ -3082,10 +3173,10 @@
         <v>43746</v>
       </c>
       <c r="B89" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C89" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -3096,10 +3187,10 @@
         <v>43781</v>
       </c>
       <c r="B90" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C90" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D90">
         <v>3</v>
@@ -3110,10 +3201,10 @@
         <v>43781</v>
       </c>
       <c r="B91" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C91" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D91">
         <v>2</v>
@@ -3124,10 +3215,10 @@
         <v>43781</v>
       </c>
       <c r="B92" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C92" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D92">
         <v>2</v>
@@ -3138,10 +3229,10 @@
         <v>43781</v>
       </c>
       <c r="B93" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C93" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D93">
         <v>0.5</v>
@@ -3152,10 +3243,10 @@
         <v>43781</v>
       </c>
       <c r="B94" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C94" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D94">
         <v>0.5</v>
@@ -3166,10 +3257,10 @@
         <v>43809</v>
       </c>
       <c r="B95" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C95" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D95">
         <v>3</v>
@@ -3180,10 +3271,10 @@
         <v>43809</v>
       </c>
       <c r="B96" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C96" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D96">
         <v>2</v>
@@ -3194,10 +3285,10 @@
         <v>43809</v>
       </c>
       <c r="B97" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C97" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D97">
         <v>0.5</v>
@@ -3208,10 +3299,10 @@
         <v>43809</v>
       </c>
       <c r="B98" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C98" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D98">
         <v>0.5</v>
@@ -3222,10 +3313,10 @@
         <v>43809</v>
       </c>
       <c r="B99" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C99" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D99">
         <v>0.5</v>
@@ -3236,10 +3327,10 @@
         <v>43809</v>
       </c>
       <c r="B100" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C100" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D100">
         <v>0.5</v>
@@ -3250,10 +3341,10 @@
         <v>43809</v>
       </c>
       <c r="B101" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C101" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D101">
         <v>0.5</v>
@@ -3264,10 +3355,10 @@
         <v>43809</v>
       </c>
       <c r="B102" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C102" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D102">
         <v>0.5</v>
@@ -3278,10 +3369,10 @@
         <v>43809</v>
       </c>
       <c r="B103" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C103" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D103">
         <v>0.5</v>
@@ -3292,10 +3383,10 @@
         <v>43809</v>
       </c>
       <c r="B104" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C104" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -3306,10 +3397,10 @@
         <v>43809</v>
       </c>
       <c r="B105" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C105" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D105">
         <v>0.5</v>
@@ -3320,10 +3411,10 @@
         <v>43844</v>
       </c>
       <c r="B106" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C106" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D106">
         <v>3</v>
@@ -3334,10 +3425,10 @@
         <v>43844</v>
       </c>
       <c r="B107" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C107" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D107">
         <v>2</v>
@@ -3348,10 +3439,10 @@
         <v>43844</v>
       </c>
       <c r="B108" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C108" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -3362,10 +3453,10 @@
         <v>43844</v>
       </c>
       <c r="B109" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C109" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D109">
         <v>0.5</v>
@@ -3376,10 +3467,10 @@
         <v>43844</v>
       </c>
       <c r="B110" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C110" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D110">
         <v>0.5</v>
@@ -3390,10 +3481,10 @@
         <v>43844</v>
       </c>
       <c r="B111" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C111" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D111">
         <v>0.5</v>
@@ -3404,10 +3495,10 @@
         <v>43844</v>
       </c>
       <c r="B112" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C112" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D112">
         <v>0.5</v>
@@ -3418,10 +3509,10 @@
         <v>43872</v>
       </c>
       <c r="B113" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C113" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D113">
         <v>3</v>
@@ -3432,10 +3523,10 @@
         <v>43872</v>
       </c>
       <c r="B114" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C114" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D114">
         <v>2</v>
@@ -3446,10 +3537,10 @@
         <v>43872</v>
       </c>
       <c r="B115" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C115" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D115">
         <v>1</v>
@@ -3460,10 +3551,10 @@
         <v>43872</v>
       </c>
       <c r="B116" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C116" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D116">
         <v>0.5</v>
@@ -3474,10 +3565,10 @@
         <v>43872</v>
       </c>
       <c r="B117" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C117" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D117">
         <v>0.5</v>
@@ -3488,10 +3579,10 @@
         <v>43872</v>
       </c>
       <c r="B118" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C118" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D118">
         <v>0.5</v>
@@ -3502,12 +3593,68 @@
         <v>43872</v>
       </c>
       <c r="B119" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C119" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D119">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="1">
+        <v>44392</v>
+      </c>
+      <c r="B120" t="s">
+        <v>39</v>
+      </c>
+      <c r="C120" t="s">
+        <v>120</v>
+      </c>
+      <c r="D120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="1">
+        <v>44392</v>
+      </c>
+      <c r="B121" t="s">
+        <v>69</v>
+      </c>
+      <c r="C121" t="s">
+        <v>102</v>
+      </c>
+      <c r="D121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="1">
+        <v>44392</v>
+      </c>
+      <c r="B122" t="s">
+        <v>141</v>
+      </c>
+      <c r="C122" t="s">
+        <v>109</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="1">
+        <v>44392</v>
+      </c>
+      <c r="B123" t="s">
+        <v>101</v>
+      </c>
+      <c r="C123" t="s">
+        <v>84</v>
+      </c>
+      <c r="D123">
         <v>0.5</v>
       </c>
     </row>
@@ -3539,10 +3686,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3552,112 +3699,117 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added first 6 months of 2022 styles
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2b05\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:40009_{60F62788-76A3-4AF9-B9B3-0AD1796CD7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D39708A-8650-4957-9FAC-E20B3FEE12FF}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="13_ncr:40009_{60F62788-76A3-4AF9-B9B3-0AD1796CD7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D623C302-D8CD-49CC-84A3-AB9CC100797A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Competitions" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="149">
   <si>
     <t>Date</t>
   </si>
@@ -141,6 +141,24 @@
   </si>
   <si>
     <t>Mead and Fruit Beers</t>
+  </si>
+  <si>
+    <t>Open/Club Brews</t>
+  </si>
+  <si>
+    <t>All Non-American Styles (European, Mexican, etc.)</t>
+  </si>
+  <si>
+    <t>Lagers and Sour/Funky Beers</t>
+  </si>
+  <si>
+    <t>American and Hoppy Beers</t>
+  </si>
+  <si>
+    <t>Open (focus on a "clone" beer)</t>
+  </si>
+  <si>
+    <t>Club Brew/Big Brew Day</t>
   </si>
   <si>
     <t>Name</t>
@@ -1018,8 +1036,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:D43" totalsRowShown="0">
-  <autoFilter ref="A1:D43" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:D49" totalsRowShown="0">
+  <autoFilter ref="A1:D49" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Style"/>
@@ -1350,10 +1368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1966,6 +1984,72 @@
         <v>2015</v>
       </c>
     </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>44572</v>
+      </c>
+      <c r="B44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>44600</v>
+      </c>
+      <c r="B45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>44628</v>
+      </c>
+      <c r="B46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>44663</v>
+      </c>
+      <c r="B47" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>44691</v>
+      </c>
+      <c r="B48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>44726</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49">
+        <v>2015</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1978,7 +2062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C106" workbookViewId="0">
+    <sheetView topLeftCell="A106" workbookViewId="0">
       <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
@@ -1995,13 +2079,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2009,10 +2093,10 @@
         <v>43109</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -2023,10 +2107,10 @@
         <v>43109</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -2037,10 +2121,10 @@
         <v>43109</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2051,7 +2135,7 @@
         <v>43109</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D5">
         <v>0.5</v>
@@ -2062,7 +2146,7 @@
         <v>43109</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D6">
         <v>0.5</v>
@@ -2073,10 +2157,10 @@
         <v>43137</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -2087,10 +2171,10 @@
         <v>43137</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -2101,10 +2185,10 @@
         <v>43137</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2115,10 +2199,10 @@
         <v>43172</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -2129,10 +2213,10 @@
         <v>43172</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -2143,10 +2227,10 @@
         <v>43172</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2157,7 +2241,7 @@
         <v>43172</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D13">
         <v>0.5</v>
@@ -2168,10 +2252,10 @@
         <v>43200</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -2182,10 +2266,10 @@
         <v>43200</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -2196,10 +2280,10 @@
         <v>43235</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -2210,10 +2294,10 @@
         <v>43235</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -2224,10 +2308,10 @@
         <v>43235</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -2238,7 +2322,7 @@
         <v>43235</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D19">
         <v>0.5</v>
@@ -2249,7 +2333,7 @@
         <v>43235</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D20">
         <v>0.5</v>
@@ -2260,7 +2344,7 @@
         <v>43235</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D21">
         <v>0.5</v>
@@ -2271,7 +2355,7 @@
         <v>43235</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D22">
         <v>0.5</v>
@@ -2282,7 +2366,7 @@
         <v>43235</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D23">
         <v>0.5</v>
@@ -2293,7 +2377,7 @@
         <v>43235</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D24">
         <v>0.5</v>
@@ -2304,10 +2388,10 @@
         <v>43263</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -2318,10 +2402,10 @@
         <v>43263</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -2332,10 +2416,10 @@
         <v>43263</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -2346,7 +2430,7 @@
         <v>43263</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D28">
         <v>0.5</v>
@@ -2357,7 +2441,7 @@
         <v>43263</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D29">
         <v>0.5</v>
@@ -2368,10 +2452,10 @@
         <v>43291</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -2382,10 +2466,10 @@
         <v>43291</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -2396,10 +2480,10 @@
         <v>43291</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -2410,10 +2494,10 @@
         <v>43326</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -2424,10 +2508,10 @@
         <v>43326</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -2438,10 +2522,10 @@
         <v>43326</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -2452,10 +2536,10 @@
         <v>43382</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -2466,7 +2550,7 @@
         <v>43326</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D37">
         <v>0.5</v>
@@ -2477,7 +2561,7 @@
         <v>43326</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D38">
         <v>0.5</v>
@@ -2488,7 +2572,7 @@
         <v>43326</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D39">
         <v>0.5</v>
@@ -2499,7 +2583,7 @@
         <v>43326</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D40">
         <v>0.5</v>
@@ -2510,7 +2594,7 @@
         <v>43326</v>
       </c>
       <c r="B41" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D41">
         <v>0.5</v>
@@ -2521,7 +2605,7 @@
         <v>43326</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D42">
         <v>0.5</v>
@@ -2532,10 +2616,10 @@
         <v>43382</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C43" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D43">
         <v>2</v>
@@ -2546,10 +2630,10 @@
         <v>43382</v>
       </c>
       <c r="B44" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -2560,10 +2644,10 @@
         <v>43382</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D45">
         <v>0.5</v>
@@ -2574,10 +2658,10 @@
         <v>43354</v>
       </c>
       <c r="B46" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D46">
         <v>3</v>
@@ -2588,10 +2672,10 @@
         <v>43473</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D47">
         <v>3</v>
@@ -2602,10 +2686,10 @@
         <v>43473</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C48" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D48">
         <v>2</v>
@@ -2616,10 +2700,10 @@
         <v>43473</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C49" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -2630,10 +2714,10 @@
         <v>43473</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D50">
         <v>0.5</v>
@@ -2644,10 +2728,10 @@
         <v>43473</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D51">
         <v>0.5</v>
@@ -2658,10 +2742,10 @@
         <v>43473</v>
       </c>
       <c r="B52" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D52">
         <v>0.5</v>
@@ -2672,10 +2756,10 @@
         <v>43508</v>
       </c>
       <c r="B53" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D53">
         <v>3</v>
@@ -2686,10 +2770,10 @@
         <v>43508</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C54" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -2700,10 +2784,10 @@
         <v>43536</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C55" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D55">
         <v>3</v>
@@ -2714,10 +2798,10 @@
         <v>43536</v>
       </c>
       <c r="B56" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C56" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D56">
         <v>2</v>
@@ -2728,10 +2812,10 @@
         <v>43536</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C57" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -2742,10 +2826,10 @@
         <v>43536</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C58" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D58">
         <v>0.5</v>
@@ -2756,10 +2840,10 @@
         <v>43536</v>
       </c>
       <c r="B59" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C59" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D59">
         <v>0.5</v>
@@ -2770,10 +2854,10 @@
         <v>43627</v>
       </c>
       <c r="B60" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C60" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D60">
         <v>3</v>
@@ -2784,10 +2868,10 @@
         <v>43627</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C61" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -2798,10 +2882,10 @@
         <v>43627</v>
       </c>
       <c r="B62" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C62" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -2812,10 +2896,10 @@
         <v>43627</v>
       </c>
       <c r="B63" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D63">
         <v>0.5</v>
@@ -2826,10 +2910,10 @@
         <v>43627</v>
       </c>
       <c r="B64" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C64" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D64">
         <v>0.5</v>
@@ -2840,10 +2924,10 @@
         <v>43627</v>
       </c>
       <c r="B65" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C65" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D65">
         <v>0.5</v>
@@ -2854,10 +2938,10 @@
         <v>43627</v>
       </c>
       <c r="B66" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C66" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D66">
         <v>0.5</v>
@@ -2868,10 +2952,10 @@
         <v>43627</v>
       </c>
       <c r="B67" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C67" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D67">
         <v>0.5</v>
@@ -2882,10 +2966,10 @@
         <v>43627</v>
       </c>
       <c r="B68" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C68" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D68">
         <v>0.5</v>
@@ -2896,10 +2980,10 @@
         <v>43627</v>
       </c>
       <c r="B69" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C69" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D69">
         <v>0.5</v>
@@ -2910,10 +2994,10 @@
         <v>43655</v>
       </c>
       <c r="B70" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C70" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D70">
         <v>3</v>
@@ -2924,10 +3008,10 @@
         <v>43655</v>
       </c>
       <c r="B71" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C71" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="D71">
         <v>2</v>
@@ -2938,10 +3022,10 @@
         <v>43655</v>
       </c>
       <c r="B72" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C72" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -2952,10 +3036,10 @@
         <v>43655</v>
       </c>
       <c r="B73" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C73" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D73">
         <v>0.5</v>
@@ -2966,10 +3050,10 @@
         <v>43690</v>
       </c>
       <c r="B74" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C74" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D74">
         <v>3</v>
@@ -2980,10 +3064,10 @@
         <v>43690</v>
       </c>
       <c r="B75" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C75" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D75">
         <v>2</v>
@@ -2994,10 +3078,10 @@
         <v>43690</v>
       </c>
       <c r="B76" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C76" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -3008,10 +3092,10 @@
         <v>43690</v>
       </c>
       <c r="B77" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C77" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D77">
         <v>0.5</v>
@@ -3022,10 +3106,10 @@
         <v>43690</v>
       </c>
       <c r="B78" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C78" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D78">
         <v>0.5</v>
@@ -3036,10 +3120,10 @@
         <v>43690</v>
       </c>
       <c r="B79" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C79" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D79">
         <v>0.5</v>
@@ -3050,10 +3134,10 @@
         <v>43690</v>
       </c>
       <c r="B80" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C80" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D80">
         <v>0.5</v>
@@ -3064,10 +3148,10 @@
         <v>43718</v>
       </c>
       <c r="B81" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C81" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D81">
         <v>3</v>
@@ -3078,10 +3162,10 @@
         <v>43718</v>
       </c>
       <c r="B82" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C82" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D82">
         <v>2</v>
@@ -3092,10 +3176,10 @@
         <v>43718</v>
       </c>
       <c r="B83" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C83" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -3106,10 +3190,10 @@
         <v>43718</v>
       </c>
       <c r="B84" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C84" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D84">
         <v>0.5</v>
@@ -3120,10 +3204,10 @@
         <v>43718</v>
       </c>
       <c r="B85" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C85" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D85">
         <v>0.5</v>
@@ -3134,10 +3218,10 @@
         <v>43718</v>
       </c>
       <c r="B86" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C86" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D86">
         <v>0.5</v>
@@ -3148,10 +3232,10 @@
         <v>43746</v>
       </c>
       <c r="B87" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C87" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D87">
         <v>3</v>
@@ -3162,10 +3246,10 @@
         <v>43746</v>
       </c>
       <c r="B88" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C88" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D88">
         <v>2</v>
@@ -3176,10 +3260,10 @@
         <v>43746</v>
       </c>
       <c r="B89" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C89" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -3190,10 +3274,10 @@
         <v>43781</v>
       </c>
       <c r="B90" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C90" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D90">
         <v>3</v>
@@ -3204,10 +3288,10 @@
         <v>43781</v>
       </c>
       <c r="B91" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C91" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D91">
         <v>2</v>
@@ -3218,10 +3302,10 @@
         <v>43781</v>
       </c>
       <c r="B92" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C92" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D92">
         <v>2</v>
@@ -3232,10 +3316,10 @@
         <v>43781</v>
       </c>
       <c r="B93" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C93" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D93">
         <v>0.5</v>
@@ -3246,10 +3330,10 @@
         <v>43781</v>
       </c>
       <c r="B94" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C94" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D94">
         <v>0.5</v>
@@ -3260,10 +3344,10 @@
         <v>43809</v>
       </c>
       <c r="B95" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C95" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D95">
         <v>3</v>
@@ -3274,10 +3358,10 @@
         <v>43809</v>
       </c>
       <c r="B96" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C96" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D96">
         <v>2</v>
@@ -3288,10 +3372,10 @@
         <v>43809</v>
       </c>
       <c r="B97" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C97" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D97">
         <v>0.5</v>
@@ -3302,10 +3386,10 @@
         <v>43809</v>
       </c>
       <c r="B98" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C98" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D98">
         <v>0.5</v>
@@ -3316,10 +3400,10 @@
         <v>43809</v>
       </c>
       <c r="B99" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C99" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D99">
         <v>0.5</v>
@@ -3330,10 +3414,10 @@
         <v>43809</v>
       </c>
       <c r="B100" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C100" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="D100">
         <v>0.5</v>
@@ -3344,10 +3428,10 @@
         <v>43809</v>
       </c>
       <c r="B101" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C101" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D101">
         <v>0.5</v>
@@ -3358,10 +3442,10 @@
         <v>43809</v>
       </c>
       <c r="B102" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C102" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D102">
         <v>0.5</v>
@@ -3372,10 +3456,10 @@
         <v>43809</v>
       </c>
       <c r="B103" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C103" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="D103">
         <v>0.5</v>
@@ -3386,10 +3470,10 @@
         <v>43809</v>
       </c>
       <c r="B104" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C104" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -3400,10 +3484,10 @@
         <v>43809</v>
       </c>
       <c r="B105" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C105" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="D105">
         <v>0.5</v>
@@ -3414,10 +3498,10 @@
         <v>43844</v>
       </c>
       <c r="B106" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C106" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D106">
         <v>3</v>
@@ -3428,10 +3512,10 @@
         <v>43844</v>
       </c>
       <c r="B107" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C107" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D107">
         <v>2</v>
@@ -3442,10 +3526,10 @@
         <v>43844</v>
       </c>
       <c r="B108" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C108" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -3456,10 +3540,10 @@
         <v>43844</v>
       </c>
       <c r="B109" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C109" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D109">
         <v>0.5</v>
@@ -3470,10 +3554,10 @@
         <v>43844</v>
       </c>
       <c r="B110" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C110" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D110">
         <v>0.5</v>
@@ -3484,10 +3568,10 @@
         <v>43844</v>
       </c>
       <c r="B111" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C111" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D111">
         <v>0.5</v>
@@ -3498,10 +3582,10 @@
         <v>43844</v>
       </c>
       <c r="B112" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C112" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D112">
         <v>0.5</v>
@@ -3512,10 +3596,10 @@
         <v>43872</v>
       </c>
       <c r="B113" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C113" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D113">
         <v>3</v>
@@ -3526,10 +3610,10 @@
         <v>43872</v>
       </c>
       <c r="B114" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C114" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D114">
         <v>2</v>
@@ -3540,10 +3624,10 @@
         <v>43872</v>
       </c>
       <c r="B115" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C115" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D115">
         <v>1</v>
@@ -3554,10 +3638,10 @@
         <v>43872</v>
       </c>
       <c r="B116" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C116" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D116">
         <v>0.5</v>
@@ -3568,10 +3652,10 @@
         <v>43872</v>
       </c>
       <c r="B117" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C117" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D117">
         <v>0.5</v>
@@ -3582,10 +3666,10 @@
         <v>43872</v>
       </c>
       <c r="B118" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C118" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D118">
         <v>0.5</v>
@@ -3596,10 +3680,10 @@
         <v>43872</v>
       </c>
       <c r="B119" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C119" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D119">
         <v>0.5</v>
@@ -3610,10 +3694,10 @@
         <v>44392</v>
       </c>
       <c r="B120" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C120" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D120">
         <v>3</v>
@@ -3624,10 +3708,10 @@
         <v>44392</v>
       </c>
       <c r="B121" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C121" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D121">
         <v>2</v>
@@ -3638,10 +3722,10 @@
         <v>44392</v>
       </c>
       <c r="B122" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C122" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D122">
         <v>1</v>
@@ -3652,10 +3736,10 @@
         <v>44392</v>
       </c>
       <c r="B123" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C123" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D123">
         <v>0.5</v>
@@ -3666,10 +3750,10 @@
         <v>44418</v>
       </c>
       <c r="B124" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C124" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="D124">
         <v>3</v>
@@ -3680,10 +3764,10 @@
         <v>44418</v>
       </c>
       <c r="B125" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C125" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D125">
         <v>2</v>
@@ -3730,117 +3814,117 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Does not like having category empty for comp data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2b05\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="13_ncr:40009_{60F62788-76A3-4AF9-B9B3-0AD1796CD7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D623C302-D8CD-49CC-84A3-AB9CC100797A}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="13_ncr:40009_{60F62788-76A3-4AF9-B9B3-0AD1796CD7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0164F045-3BB9-419C-9C7D-4671EDB2F50C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Competitions" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="149">
   <si>
     <t>Date</t>
   </si>
@@ -1371,7 +1371,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1991,6 +1991,9 @@
       <c r="B44" t="s">
         <v>36</v>
       </c>
+      <c r="C44" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D44">
         <v>2015</v>
       </c>
@@ -2002,6 +2005,9 @@
       <c r="B45" t="s">
         <v>37</v>
       </c>
+      <c r="C45" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D45">
         <v>2015</v>
       </c>
@@ -2013,6 +2019,9 @@
       <c r="B46" t="s">
         <v>38</v>
       </c>
+      <c r="C46" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D46">
         <v>2015</v>
       </c>
@@ -2024,6 +2033,9 @@
       <c r="B47" t="s">
         <v>39</v>
       </c>
+      <c r="C47" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D47">
         <v>2015</v>
       </c>
@@ -2035,6 +2047,9 @@
       <c r="B48" t="s">
         <v>40</v>
       </c>
+      <c r="C48" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="D48">
         <v>2015</v>
       </c>
@@ -2045,6 +2060,9 @@
       </c>
       <c r="B49" t="s">
         <v>41</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D49">
         <v>2015</v>

</xml_diff>

<commit_message>
Added last 6 months of 2022 comps
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb7610fc81a54cae/ABL/ABL 3.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="13_ncr:40009_{60F62788-76A3-4AF9-B9B3-0AD1796CD7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E140C33-B441-45E4-A728-38D6D47D5B2A}"/>
+  <xr:revisionPtr revIDLastSave="238" documentId="13_ncr:40009_{60F62788-76A3-4AF9-B9B3-0AD1796CD7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30D24395-A598-4861-A65B-3FE2CF1A03D4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Competitions" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="161">
   <si>
     <t>Date</t>
   </si>
@@ -498,6 +498,24 @@
   </si>
   <si>
     <t>Best Bitter</t>
+  </si>
+  <si>
+    <t>Club Yeast Beers</t>
+  </si>
+  <si>
+    <t>Meads, Cysers, Ciders</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>SHIVs, Darks (NOT Porters or Stouts)</t>
+  </si>
+  <si>
+    <t>Porters, Stouts, Big Beers</t>
+  </si>
+  <si>
+    <t>Session Beers (under 5% ABV)</t>
   </si>
 </sst>
 </file>
@@ -1054,8 +1072,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:D49" totalsRowShown="0">
-  <autoFilter ref="A1:D49" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:D55" totalsRowShown="0">
+  <autoFilter ref="A1:D55" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Style"/>
@@ -1386,21 +1404,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1414,7 +1432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43109</v>
       </c>
@@ -1428,7 +1446,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43137</v>
       </c>
@@ -1442,7 +1460,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43172</v>
       </c>
@@ -1456,7 +1474,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>43200</v>
       </c>
@@ -1470,7 +1488,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43235</v>
       </c>
@@ -1484,7 +1502,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43263</v>
       </c>
@@ -1498,7 +1516,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>43291</v>
       </c>
@@ -1512,7 +1530,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>43326</v>
       </c>
@@ -1526,7 +1544,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>43382</v>
       </c>
@@ -1540,7 +1558,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>43354</v>
       </c>
@@ -1554,7 +1572,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>43417</v>
       </c>
@@ -1568,7 +1586,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>43445</v>
       </c>
@@ -1582,7 +1600,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>43473</v>
       </c>
@@ -1596,7 +1614,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>43508</v>
       </c>
@@ -1610,7 +1628,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>43536</v>
       </c>
@@ -1624,7 +1642,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>43564</v>
       </c>
@@ -1638,7 +1656,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>43599</v>
       </c>
@@ -1652,7 +1670,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>43627</v>
       </c>
@@ -1666,7 +1684,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>43655</v>
       </c>
@@ -1680,7 +1698,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>43690</v>
       </c>
@@ -1694,7 +1712,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43718</v>
       </c>
@@ -1708,7 +1726,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>43746</v>
       </c>
@@ -1722,7 +1740,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>43781</v>
       </c>
@@ -1736,7 +1754,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>43809</v>
       </c>
@@ -1750,7 +1768,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>43844</v>
       </c>
@@ -1764,7 +1782,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>43872</v>
       </c>
@@ -1778,7 +1796,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>43900</v>
       </c>
@@ -1792,7 +1810,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>43935</v>
       </c>
@@ -1806,7 +1824,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>43963</v>
       </c>
@@ -1820,7 +1838,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>43991</v>
       </c>
@@ -1834,7 +1852,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>44026</v>
       </c>
@@ -1848,7 +1866,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>44054</v>
       </c>
@@ -1862,7 +1880,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>44082</v>
       </c>
@@ -1876,7 +1894,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>44117</v>
       </c>
@@ -1890,7 +1908,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>44145</v>
       </c>
@@ -1904,7 +1922,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>44173</v>
       </c>
@@ -1918,7 +1936,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>44392</v>
       </c>
@@ -1932,7 +1950,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>44418</v>
       </c>
@@ -1946,7 +1964,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>44453</v>
       </c>
@@ -1960,7 +1978,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>44481</v>
       </c>
@@ -1974,7 +1992,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>44509</v>
       </c>
@@ -1988,7 +2006,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>44544</v>
       </c>
@@ -2002,7 +2020,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>44572</v>
       </c>
@@ -2016,7 +2034,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44600</v>
       </c>
@@ -2030,7 +2048,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44628</v>
       </c>
@@ -2044,7 +2062,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>44663</v>
       </c>
@@ -2058,7 +2076,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>44691</v>
       </c>
@@ -2072,7 +2090,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>44726</v>
       </c>
@@ -2083,6 +2101,72 @@
         <v>13</v>
       </c>
       <c r="D49">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>44754</v>
+      </c>
+      <c r="B50" t="s">
+        <v>160</v>
+      </c>
+      <c r="D50">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>44782</v>
+      </c>
+      <c r="B51" t="s">
+        <v>155</v>
+      </c>
+      <c r="D51">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>44817</v>
+      </c>
+      <c r="B52" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>44845</v>
+      </c>
+      <c r="B53" t="s">
+        <v>157</v>
+      </c>
+      <c r="D53">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>44873</v>
+      </c>
+      <c r="B54" t="s">
+        <v>158</v>
+      </c>
+      <c r="D54">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>44908</v>
+      </c>
+      <c r="B55" t="s">
+        <v>159</v>
+      </c>
+      <c r="D55">
         <v>2015</v>
       </c>
     </row>
@@ -2098,19 +2182,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+    <sheetView topLeftCell="A127" workbookViewId="0">
       <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2124,7 +2208,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43109</v>
       </c>
@@ -2138,7 +2222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43109</v>
       </c>
@@ -2152,7 +2236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43109</v>
       </c>
@@ -2166,7 +2250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>43109</v>
       </c>
@@ -2177,7 +2261,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43109</v>
       </c>
@@ -2188,7 +2272,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43137</v>
       </c>
@@ -2202,7 +2286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>43137</v>
       </c>
@@ -2216,7 +2300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>43137</v>
       </c>
@@ -2230,7 +2314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>43172</v>
       </c>
@@ -2244,7 +2328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>43172</v>
       </c>
@@ -2258,7 +2342,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>43172</v>
       </c>
@@ -2272,7 +2356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>43172</v>
       </c>
@@ -2283,7 +2367,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>43200</v>
       </c>
@@ -2297,7 +2381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>43200</v>
       </c>
@@ -2311,7 +2395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>43235</v>
       </c>
@@ -2325,7 +2409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>43235</v>
       </c>
@@ -2339,7 +2423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>43235</v>
       </c>
@@ -2353,7 +2437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>43235</v>
       </c>
@@ -2364,7 +2448,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>43235</v>
       </c>
@@ -2375,7 +2459,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>43235</v>
       </c>
@@ -2386,7 +2470,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43235</v>
       </c>
@@ -2397,7 +2481,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>43235</v>
       </c>
@@ -2408,7 +2492,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>43235</v>
       </c>
@@ -2419,7 +2503,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>43263</v>
       </c>
@@ -2433,7 +2517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>43263</v>
       </c>
@@ -2447,7 +2531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>43263</v>
       </c>
@@ -2461,7 +2545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>43263</v>
       </c>
@@ -2472,7 +2556,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>43263</v>
       </c>
@@ -2483,7 +2567,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>43291</v>
       </c>
@@ -2497,7 +2581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>43291</v>
       </c>
@@ -2511,7 +2595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>43291</v>
       </c>
@@ -2525,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>43326</v>
       </c>
@@ -2539,7 +2623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>43326</v>
       </c>
@@ -2553,7 +2637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>43326</v>
       </c>
@@ -2567,7 +2651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>43382</v>
       </c>
@@ -2581,7 +2665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>43326</v>
       </c>
@@ -2592,7 +2676,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>43326</v>
       </c>
@@ -2603,7 +2687,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>43326</v>
       </c>
@@ -2614,7 +2698,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>43326</v>
       </c>
@@ -2625,7 +2709,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>43326</v>
       </c>
@@ -2636,7 +2720,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>43326</v>
       </c>
@@ -2647,7 +2731,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>43382</v>
       </c>
@@ -2661,7 +2745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43382</v>
       </c>
@@ -2675,7 +2759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43382</v>
       </c>
@@ -2689,7 +2773,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>43354</v>
       </c>
@@ -2703,7 +2787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>43473</v>
       </c>
@@ -2717,7 +2801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>43473</v>
       </c>
@@ -2731,7 +2815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>43473</v>
       </c>
@@ -2745,7 +2829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>43473</v>
       </c>
@@ -2759,7 +2843,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>43473</v>
       </c>
@@ -2773,7 +2857,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>43473</v>
       </c>
@@ -2787,7 +2871,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>43508</v>
       </c>
@@ -2801,7 +2885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>43508</v>
       </c>
@@ -2815,7 +2899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>43536</v>
       </c>
@@ -2829,7 +2913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>43536</v>
       </c>
@@ -2843,7 +2927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>43536</v>
       </c>
@@ -2857,7 +2941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>43536</v>
       </c>
@@ -2871,7 +2955,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>43536</v>
       </c>
@@ -2885,7 +2969,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>43627</v>
       </c>
@@ -2899,7 +2983,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>43627</v>
       </c>
@@ -2913,7 +2997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>43627</v>
       </c>
@@ -2927,7 +3011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>43627</v>
       </c>
@@ -2941,7 +3025,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>43627</v>
       </c>
@@ -2955,7 +3039,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>43627</v>
       </c>
@@ -2969,7 +3053,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>43627</v>
       </c>
@@ -2983,7 +3067,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>43627</v>
       </c>
@@ -2997,7 +3081,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>43627</v>
       </c>
@@ -3011,7 +3095,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>43627</v>
       </c>
@@ -3025,7 +3109,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>43655</v>
       </c>
@@ -3039,7 +3123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>43655</v>
       </c>
@@ -3053,7 +3137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>43655</v>
       </c>
@@ -3067,7 +3151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>43655</v>
       </c>
@@ -3081,7 +3165,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>43690</v>
       </c>
@@ -3095,7 +3179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>43690</v>
       </c>
@@ -3109,7 +3193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>43690</v>
       </c>
@@ -3123,7 +3207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>43690</v>
       </c>
@@ -3137,7 +3221,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>43690</v>
       </c>
@@ -3151,7 +3235,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>43690</v>
       </c>
@@ -3165,7 +3249,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>43690</v>
       </c>
@@ -3179,7 +3263,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>43718</v>
       </c>
@@ -3193,7 +3277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>43718</v>
       </c>
@@ -3207,7 +3291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>43718</v>
       </c>
@@ -3221,7 +3305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>43718</v>
       </c>
@@ -3235,7 +3319,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>43718</v>
       </c>
@@ -3249,7 +3333,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>43718</v>
       </c>
@@ -3263,7 +3347,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>43746</v>
       </c>
@@ -3277,7 +3361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>43746</v>
       </c>
@@ -3291,7 +3375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>43746</v>
       </c>
@@ -3305,7 +3389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>43781</v>
       </c>
@@ -3319,7 +3403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>43781</v>
       </c>
@@ -3333,7 +3417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>43781</v>
       </c>
@@ -3347,7 +3431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>43781</v>
       </c>
@@ -3361,7 +3445,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>43781</v>
       </c>
@@ -3375,7 +3459,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>43809</v>
       </c>
@@ -3389,7 +3473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>43809</v>
       </c>
@@ -3403,7 +3487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>43809</v>
       </c>
@@ -3417,7 +3501,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>43809</v>
       </c>
@@ -3431,7 +3515,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>43809</v>
       </c>
@@ -3445,7 +3529,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>43809</v>
       </c>
@@ -3459,7 +3543,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>43809</v>
       </c>
@@ -3473,7 +3557,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>43809</v>
       </c>
@@ -3487,7 +3571,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>43809</v>
       </c>
@@ -3501,7 +3585,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>43809</v>
       </c>
@@ -3515,7 +3599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>43809</v>
       </c>
@@ -3529,7 +3613,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>43844</v>
       </c>
@@ -3543,7 +3627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>43844</v>
       </c>
@@ -3557,7 +3641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>43844</v>
       </c>
@@ -3571,7 +3655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>43844</v>
       </c>
@@ -3585,7 +3669,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>43844</v>
       </c>
@@ -3599,7 +3683,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>43844</v>
       </c>
@@ -3613,7 +3697,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>43844</v>
       </c>
@@ -3627,7 +3711,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>43872</v>
       </c>
@@ -3641,7 +3725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>43872</v>
       </c>
@@ -3655,7 +3739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>43872</v>
       </c>
@@ -3669,7 +3753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>43872</v>
       </c>
@@ -3683,7 +3767,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>43872</v>
       </c>
@@ -3697,7 +3781,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>43872</v>
       </c>
@@ -3711,7 +3795,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>43872</v>
       </c>
@@ -3725,7 +3809,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>44392</v>
       </c>
@@ -3739,7 +3823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>44392</v>
       </c>
@@ -3753,7 +3837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>44392</v>
       </c>
@@ -3767,7 +3851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>44392</v>
       </c>
@@ -3781,7 +3865,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>44418</v>
       </c>
@@ -3795,7 +3879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>44418</v>
       </c>
@@ -3809,7 +3893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>44509</v>
       </c>
@@ -3823,7 +3907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>44509</v>
       </c>
@@ -3837,7 +3921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>44509</v>
       </c>
@@ -3851,7 +3935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>44509</v>
       </c>
@@ -3865,7 +3949,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>44509</v>
       </c>
@@ -3879,7 +3963,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>44509</v>
       </c>
@@ -3893,7 +3977,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>44509</v>
       </c>
@@ -3907,7 +3991,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>44509</v>
       </c>
@@ -3921,7 +4005,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>44572</v>
       </c>
@@ -3935,7 +4019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>44572</v>
       </c>
@@ -3949,7 +4033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>44572</v>
       </c>
@@ -3963,7 +4047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>44572</v>
       </c>
@@ -3977,7 +4061,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>44572</v>
       </c>
@@ -3991,7 +4075,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>44572</v>
       </c>
@@ -4005,7 +4089,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>44600</v>
       </c>
@@ -4019,7 +4103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>44600</v>
       </c>
@@ -4033,7 +4117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>44600</v>
       </c>
@@ -4047,7 +4131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>44600</v>
       </c>
@@ -4061,7 +4145,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>44600</v>
       </c>
@@ -4109,122 +4193,122 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>147</v>
       </c>

</xml_diff>